<commit_message>
Stats being used and its ok
</commit_message>
<xml_diff>
--- a/ASD Tests.xlsx
+++ b/ASD Tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23513"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60B8406E-27E5-4EDF-8574-A1CFF0962313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABBAEE06-D78B-44D8-9570-2669E6F850ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="15">
   <si>
     <t>Broadcast</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Total Messages/Bytes Received</t>
   </si>
   <si>
-    <t>Sucess Rate(%)</t>
-  </si>
-  <si>
     <t>Average Broadcast reliability</t>
   </si>
   <si>
@@ -67,7 +64,7 @@
     <t>1K</t>
   </si>
   <si>
-    <t>1M</t>
+    <t>100K</t>
   </si>
   <si>
     <t>Cyclon</t>
@@ -439,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -451,12 +448,12 @@
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="9" width="28.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" customWidth="1"/>
+    <col min="7" max="8" width="28.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,730 +481,581 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <f>(G3/C3) * 100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>200</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H37" si="0">(G4/C4) * 100</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>2000</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>2000</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D7">
         <v>200</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D8">
         <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <v>2000</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D10">
         <v>2000</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>200</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <v>200</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>2000</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>2000</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D17">
         <v>200</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D18">
         <v>2000</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D19">
         <v>2000</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D21">
         <v>200</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D22">
         <v>200</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D23">
         <v>2000</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D24">
         <v>2000</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D25">
         <v>200</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D26">
         <v>200</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D27">
         <v>2000</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D28">
         <v>2000</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D30">
         <v>200</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>200</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>2000</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D33">
         <v>2000</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D34">
         <v>200</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D35">
         <v>200</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D36">
         <v>2000</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C37">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D37">
         <v>2000</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>